<commit_message>
update cron del export/file device2&device3
</commit_message>
<xml_diff>
--- a/runtime/export/device3.xlsx
+++ b/runtime/export/device3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21323" windowHeight="10127"/>
+    <workbookView windowWidth="21323" windowHeight="10535"/>
   </bookViews>
   <sheets>
     <sheet name="设备基本信息表" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502">
   <si>
     <t>资产编号</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>人员姓名</t>
+  </si>
+  <si>
+    <t>设备位置</t>
   </si>
   <si>
     <t>设备类型代码</t>
@@ -1540,10 +1543,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1586,7 +1589,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1618,29 +1636,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1707,6 +1702,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -1730,25 +1733,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1778,30 +1781,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1815,6 +1794,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1874,6 +1859,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1921,21 +1924,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2013,6 +2001,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2029,145 +2032,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2536,10 +2539,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -2553,10 +2556,11 @@
     <col min="7" max="7" width="23.1111111111111" style="4" customWidth="1"/>
     <col min="8" max="8" width="14.3888888888889" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.1111111111111" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="4"/>
+    <col min="10" max="10" width="9.22222222222222" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2583,6 +2587,9 @@
       </c>
       <c r="I1" s="6" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="9:9">
@@ -2614,2719 +2621,2719 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="1" spans="1:3">
       <c r="A104" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="C205" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="3" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="3" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" s="3" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="3" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C242" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="3" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C244" s="3" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="3" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="3" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>